<commit_message>
Update to account for degrees of freedom in test
</commit_message>
<xml_diff>
--- a/Stroop Effect.xlsx
+++ b/Stroop Effect.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Congruent</t>
   </si>
@@ -112,6 +112,15 @@
   </si>
   <si>
     <t>Stderror of differences:</t>
+  </si>
+  <si>
+    <t>Calculate SE alternate way:</t>
+  </si>
+  <si>
+    <t>Alternate T-value:</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -1889,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView tabSelected="1" topLeftCell="B21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2578,8 +2587,23 @@
         <v>8.020706944109957</v>
       </c>
     </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44">
+        <f>SQRT((S22+S5)/S19)</f>
+        <v>0.59007114966877527</v>
+      </c>
+    </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="11"/>
+      <c r="G45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H45" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="11"/>

</xml_diff>